<commit_message>
Fixed typos in WU for R, addressed irregularities in SWC code and in WU code
</commit_message>
<xml_diff>
--- a/input/Average empty pot weight calculations.xlsx
+++ b/input/Average empty pot weight calculations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Documents\Forrestel Lab\GH Drydown\Data\Data for uploading to github\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\imnik\Documents\GitHub\vitisdrought\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{424D9878-1CEF-4D68-94BF-8137BB49463A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81C24E9A-B757-4678-87BC-A25B9F507165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="emptypots" sheetId="1" r:id="rId1"/>
@@ -1106,11 +1106,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M21" sqref="M21:N21"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="Z21" sqref="Z21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="5.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.90625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="27.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.36328125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="105.7265625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.36328125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.90625" bestFit="1" customWidth="1"/>
+    <col min="21" max="24" width="19.36328125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="34.453125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="94.7265625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="19.36328125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="37.453125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -2438,7 +2464,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7393E51-1278-4A8C-8A35-BF2BD6CF7312}">
   <dimension ref="B2:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>

</xml_diff>